<commit_message>
Add confusion matrix plotting
</commit_message>
<xml_diff>
--- a/Statisticki podaci modela.xlsx
+++ b/Statisticki podaci modela.xlsx
@@ -31,22 +31,22 @@
     <t>Tocnost</t>
   </si>
   <si>
-    <t>TP</t>
-  </si>
-  <si>
-    <t>FP</t>
-  </si>
-  <si>
-    <t>FN</t>
-  </si>
-  <si>
-    <t>TN</t>
-  </si>
-  <si>
-    <t>FPR</t>
-  </si>
-  <si>
-    <t>TNR</t>
+    <t>True Positive</t>
+  </si>
+  <si>
+    <t>False Positive</t>
+  </si>
+  <si>
+    <t>False Negative</t>
+  </si>
+  <si>
+    <t>True Negative</t>
+  </si>
+  <si>
+    <t>False Positive Rate</t>
+  </si>
+  <si>
+    <t>True Negative Rate</t>
   </si>
   <si>
     <t>Opoziv</t>
@@ -609,34 +609,34 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>2.101980924606323</v>
+        <v>11.24628973007202</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E2">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F2">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G2">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H2">
-        <v>3981</v>
+        <v>3985</v>
       </c>
       <c r="I2">
-        <v>0.475</v>
+        <v>0.375</v>
       </c>
       <c r="J2">
-        <v>99.52499999999999</v>
+        <v>99.625</v>
       </c>
       <c r="K2">
-        <v>76.25</v>
+        <v>73.75</v>
       </c>
       <c r="L2">
-        <v>82.98235478732259</v>
+        <v>81.40699538055453</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -644,7 +644,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.02349591255187988</v>
+        <v>0.07761979103088379</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>14</v>
@@ -653,25 +653,25 @@
         <v>70</v>
       </c>
       <c r="F3">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G3">
         <v>10</v>
       </c>
       <c r="H3">
-        <v>3993</v>
+        <v>3990</v>
       </c>
       <c r="I3">
-        <v>0.175</v>
+        <v>0.25</v>
       </c>
       <c r="J3">
-        <v>99.825</v>
+        <v>99.75</v>
       </c>
       <c r="K3">
         <v>87.5</v>
       </c>
       <c r="L3">
-        <v>89.22466436956677</v>
+        <v>89.13783048991817</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -679,7 +679,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>90.93137254901961</v>
+        <v>90.80882352941177</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>15</v>
@@ -688,25 +688,25 @@
         <v>71</v>
       </c>
       <c r="F4">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G4">
         <v>9</v>
       </c>
       <c r="H4">
-        <v>3985</v>
+        <v>3987</v>
       </c>
       <c r="I4">
-        <v>0.375</v>
+        <v>0.325</v>
       </c>
       <c r="J4">
-        <v>99.625</v>
+        <v>99.675</v>
       </c>
       <c r="K4">
         <v>88.75</v>
       </c>
       <c r="L4">
-        <v>89.87002637683901</v>
+        <v>89.78193243555178</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -714,34 +714,34 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>91.01868357559768</v>
+        <v>90.83814457951738</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E5">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H5">
-        <v>3992</v>
+        <v>3991</v>
       </c>
       <c r="I5">
-        <v>0.2</v>
+        <v>0.225</v>
       </c>
       <c r="J5">
-        <v>99.8</v>
+        <v>99.77500000000001</v>
       </c>
       <c r="K5">
-        <v>96.25</v>
+        <v>95</v>
       </c>
       <c r="L5">
-        <v>93.56127385404265</v>
+        <v>92.87246979977959</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -749,28 +749,28 @@
         <v>17</v>
       </c>
       <c r="E6">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F6">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G6">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="H6">
-        <v>3992</v>
+        <v>3988</v>
       </c>
       <c r="I6">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="J6">
-        <v>99.8</v>
+        <v>99.7</v>
       </c>
       <c r="K6">
-        <v>78.75</v>
+        <v>72.5</v>
       </c>
       <c r="L6">
-        <v>84.44103094416168</v>
+        <v>80.63965093969686</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -778,13 +778,13 @@
         <v>18</v>
       </c>
       <c r="E7">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F7">
         <v>10</v>
       </c>
       <c r="G7">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="H7">
         <v>3990</v>
@@ -796,10 +796,10 @@
         <v>99.75</v>
       </c>
       <c r="K7">
-        <v>88.75</v>
+        <v>81.25</v>
       </c>
       <c r="L7">
-        <v>89.87002637683901</v>
+        <v>85.77696348716697</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -807,28 +807,28 @@
         <v>19</v>
       </c>
       <c r="E8">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F8">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H8">
-        <v>3995</v>
+        <v>3993</v>
       </c>
       <c r="I8">
-        <v>0.125</v>
+        <v>0.175</v>
       </c>
       <c r="J8">
-        <v>99.875</v>
+        <v>99.825</v>
       </c>
       <c r="K8">
-        <v>97.5</v>
+        <v>98.75</v>
       </c>
       <c r="L8">
-        <v>94.14792720067018</v>
+        <v>94.62898428720069</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -836,28 +836,28 @@
         <v>20</v>
       </c>
       <c r="E9">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G9">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H9">
-        <v>3996</v>
+        <v>3995</v>
       </c>
       <c r="I9">
-        <v>0.1</v>
+        <v>0.125</v>
       </c>
       <c r="J9">
-        <v>99.90000000000001</v>
+        <v>99.875</v>
       </c>
       <c r="K9">
-        <v>88.75</v>
+        <v>86.25</v>
       </c>
       <c r="L9">
-        <v>89.87002637683901</v>
+        <v>88.48463558739631</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -868,25 +868,25 @@
         <v>74</v>
       </c>
       <c r="F10">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G10">
         <v>6</v>
       </c>
       <c r="H10">
-        <v>3993</v>
+        <v>3996</v>
       </c>
       <c r="I10">
-        <v>0.175</v>
+        <v>0.1</v>
       </c>
       <c r="J10">
-        <v>99.825</v>
+        <v>99.90000000000001</v>
       </c>
       <c r="K10">
         <v>92.5</v>
       </c>
       <c r="L10">
-        <v>91.75336338193179</v>
+        <v>91.6615404053139</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -894,28 +894,28 @@
         <v>22</v>
       </c>
       <c r="E11">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F11">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="G11">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H11">
-        <v>3993</v>
+        <v>3986</v>
       </c>
       <c r="I11">
-        <v>0.175</v>
+        <v>0.35</v>
       </c>
       <c r="J11">
-        <v>99.825</v>
+        <v>99.65000000000001</v>
       </c>
       <c r="K11">
-        <v>92.5</v>
+        <v>90</v>
       </c>
       <c r="L11">
-        <v>91.75336338193179</v>
+        <v>90.41712998290244</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -923,28 +923,28 @@
         <v>23</v>
       </c>
       <c r="E12">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F12">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G12">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H12">
-        <v>3993</v>
+        <v>3991</v>
       </c>
       <c r="I12">
-        <v>0.175</v>
+        <v>0.225</v>
       </c>
       <c r="J12">
-        <v>99.825</v>
+        <v>99.77500000000001</v>
       </c>
       <c r="K12">
-        <v>82.5</v>
+        <v>81.25</v>
       </c>
       <c r="L12">
-        <v>86.5502347096278</v>
+        <v>85.77696348716697</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -952,28 +952,28 @@
         <v>24</v>
       </c>
       <c r="E13">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F13">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H13">
-        <v>3988</v>
+        <v>3985</v>
       </c>
       <c r="I13">
-        <v>0.3</v>
+        <v>0.375</v>
       </c>
       <c r="J13">
-        <v>99.7</v>
+        <v>99.625</v>
       </c>
       <c r="K13">
-        <v>97.5</v>
+        <v>98.75</v>
       </c>
       <c r="L13">
-        <v>94.14792720067018</v>
+        <v>94.62898428720069</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -981,28 +981,28 @@
         <v>25</v>
       </c>
       <c r="E14">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F14">
+        <v>4</v>
+      </c>
+      <c r="G14">
         <v>3</v>
       </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
       <c r="H14">
-        <v>3997</v>
+        <v>3996</v>
       </c>
       <c r="I14">
-        <v>0.075</v>
+        <v>0.1</v>
       </c>
       <c r="J14">
-        <v>99.925</v>
+        <v>99.90000000000001</v>
       </c>
       <c r="K14">
-        <v>98.75</v>
+        <v>96.25</v>
       </c>
       <c r="L14">
-        <v>94.72685201517675</v>
+        <v>93.46579854569535</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1010,28 +1010,28 @@
         <v>26</v>
       </c>
       <c r="E15">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F15">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G15">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H15">
-        <v>3992</v>
+        <v>3991</v>
       </c>
       <c r="I15">
-        <v>0.2</v>
+        <v>0.225</v>
       </c>
       <c r="J15">
-        <v>99.8</v>
+        <v>99.77500000000001</v>
       </c>
       <c r="K15">
-        <v>83.75</v>
+        <v>82.5</v>
       </c>
       <c r="L15">
-        <v>87.23318838937175</v>
+        <v>86.46852596685443</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1042,25 +1042,25 @@
         <v>79</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G16">
         <v>1</v>
       </c>
       <c r="H16">
-        <v>3996</v>
+        <v>3995</v>
       </c>
       <c r="I16">
-        <v>0.1</v>
+        <v>0.125</v>
       </c>
       <c r="J16">
-        <v>99.90000000000001</v>
+        <v>99.875</v>
       </c>
       <c r="K16">
         <v>98.75</v>
       </c>
       <c r="L16">
-        <v>94.72685201517675</v>
+        <v>94.62898428720069</v>
       </c>
     </row>
     <row r="17" spans="4:12">
@@ -1068,28 +1068,28 @@
         <v>28</v>
       </c>
       <c r="E17">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F17">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G17">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H17">
-        <v>3997</v>
+        <v>3993</v>
       </c>
       <c r="I17">
-        <v>0.075</v>
+        <v>0.175</v>
       </c>
       <c r="J17">
-        <v>99.925</v>
+        <v>99.825</v>
       </c>
       <c r="K17">
-        <v>83.75</v>
+        <v>78.75</v>
       </c>
       <c r="L17">
-        <v>87.23318838937175</v>
+        <v>84.36325432268436</v>
       </c>
     </row>
     <row r="18" spans="4:12">
@@ -1097,28 +1097,28 @@
         <v>29</v>
       </c>
       <c r="E18">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F18">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="G18">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H18">
-        <v>3978</v>
+        <v>3993</v>
       </c>
       <c r="I18">
-        <v>0.5499999999999999</v>
+        <v>0.175</v>
       </c>
       <c r="J18">
-        <v>99.45</v>
+        <v>99.825</v>
       </c>
       <c r="K18">
-        <v>93.75</v>
+        <v>92.5</v>
       </c>
       <c r="L18">
-        <v>92.36415414218204</v>
+        <v>91.6615404053139</v>
       </c>
     </row>
     <row r="19" spans="4:12">
@@ -1129,25 +1129,25 @@
         <v>80</v>
       </c>
       <c r="F19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19">
-        <v>3998</v>
+        <v>3999</v>
       </c>
       <c r="I19">
-        <v>0.05</v>
+        <v>0.025</v>
       </c>
       <c r="J19">
-        <v>99.95</v>
+        <v>99.97500000000001</v>
       </c>
       <c r="K19">
         <v>100</v>
       </c>
       <c r="L19">
-        <v>95.29820002091688</v>
+        <v>95.19914876521705</v>
       </c>
     </row>
     <row r="20" spans="4:12">
@@ -1158,25 +1158,25 @@
         <v>80</v>
       </c>
       <c r="F20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
       <c r="H20">
-        <v>3996</v>
+        <v>3997</v>
       </c>
       <c r="I20">
-        <v>0.1</v>
+        <v>0.075</v>
       </c>
       <c r="J20">
-        <v>99.90000000000001</v>
+        <v>99.925</v>
       </c>
       <c r="K20">
         <v>100</v>
       </c>
       <c r="L20">
-        <v>95.29820002091688</v>
+        <v>95.19914876521705</v>
       </c>
     </row>
     <row r="21" spans="4:12">
@@ -1184,28 +1184,28 @@
         <v>32</v>
       </c>
       <c r="E21">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F21">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21">
-        <v>3991</v>
+        <v>3992</v>
       </c>
       <c r="I21">
-        <v>0.225</v>
+        <v>0.2</v>
       </c>
       <c r="J21">
-        <v>99.77500000000001</v>
+        <v>99.8</v>
       </c>
       <c r="K21">
-        <v>98.75</v>
+        <v>100</v>
       </c>
       <c r="L21">
-        <v>94.72685201517675</v>
+        <v>95.19914876521705</v>
       </c>
     </row>
     <row r="22" spans="4:12">
@@ -1213,28 +1213,28 @@
         <v>33</v>
       </c>
       <c r="E22">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F22">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G22">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H22">
-        <v>3988</v>
+        <v>3991</v>
       </c>
       <c r="I22">
-        <v>0.3</v>
+        <v>0.225</v>
       </c>
       <c r="J22">
-        <v>99.7</v>
+        <v>99.77500000000001</v>
       </c>
       <c r="K22">
-        <v>92.5</v>
+        <v>93.75</v>
       </c>
       <c r="L22">
-        <v>91.75336338193179</v>
+        <v>92.2711052080723</v>
       </c>
     </row>
     <row r="23" spans="4:12">
@@ -1242,28 +1242,28 @@
         <v>34</v>
       </c>
       <c r="E23">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F23">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H23">
-        <v>3991</v>
+        <v>3995</v>
       </c>
       <c r="I23">
-        <v>0.225</v>
+        <v>0.125</v>
       </c>
       <c r="J23">
-        <v>99.77500000000001</v>
+        <v>99.875</v>
       </c>
       <c r="K23">
-        <v>95</v>
+        <v>97.5</v>
       </c>
       <c r="L23">
-        <v>92.96673617376446</v>
+        <v>94.05125144751109</v>
       </c>
     </row>
     <row r="24" spans="4:12">
@@ -1271,28 +1271,28 @@
         <v>35</v>
       </c>
       <c r="E24">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H24">
-        <v>3999</v>
+        <v>4000</v>
       </c>
       <c r="I24">
-        <v>0.025</v>
+        <v>0</v>
       </c>
       <c r="J24">
-        <v>99.97500000000001</v>
+        <v>100</v>
       </c>
       <c r="K24">
-        <v>96.25</v>
+        <v>97.5</v>
       </c>
       <c r="L24">
-        <v>93.56127385404265</v>
+        <v>94.05125144751109</v>
       </c>
     </row>
     <row r="25" spans="4:12">
@@ -1300,13 +1300,13 @@
         <v>36</v>
       </c>
       <c r="E25">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F25">
         <v>10</v>
       </c>
       <c r="G25">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H25">
         <v>3990</v>
@@ -1318,10 +1318,10 @@
         <v>99.75</v>
       </c>
       <c r="K25">
-        <v>88.75</v>
+        <v>87.5</v>
       </c>
       <c r="L25">
-        <v>89.87002637683901</v>
+        <v>89.13783048991817</v>
       </c>
     </row>
     <row r="26" spans="4:12">
@@ -1329,28 +1329,28 @@
         <v>37</v>
       </c>
       <c r="E26">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F26">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G26">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H26">
-        <v>3993</v>
+        <v>3994</v>
       </c>
       <c r="I26">
-        <v>0.175</v>
+        <v>0.15</v>
       </c>
       <c r="J26">
-        <v>99.825</v>
+        <v>99.85000000000001</v>
       </c>
       <c r="K26">
-        <v>93.75</v>
+        <v>98.75</v>
       </c>
       <c r="L26">
-        <v>92.36415414218204</v>
+        <v>94.62898428720069</v>
       </c>
     </row>
     <row r="27" spans="4:12">
@@ -1361,25 +1361,25 @@
         <v>67</v>
       </c>
       <c r="F27">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G27">
         <v>13</v>
       </c>
       <c r="H27">
-        <v>3983</v>
+        <v>3977</v>
       </c>
       <c r="I27">
-        <v>0.425</v>
+        <v>0.575</v>
       </c>
       <c r="J27">
-        <v>99.575</v>
+        <v>99.425</v>
       </c>
       <c r="K27">
         <v>83.75</v>
       </c>
       <c r="L27">
-        <v>87.23318838937175</v>
+        <v>87.15018567677834</v>
       </c>
     </row>
     <row r="28" spans="4:12">
@@ -1387,28 +1387,28 @@
         <v>39</v>
       </c>
       <c r="E28">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F28">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G28">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H28">
-        <v>3985</v>
+        <v>3983</v>
       </c>
       <c r="I28">
-        <v>0.375</v>
+        <v>0.425</v>
       </c>
       <c r="J28">
-        <v>99.625</v>
+        <v>99.575</v>
       </c>
       <c r="K28">
-        <v>62.5</v>
+        <v>67.5</v>
       </c>
       <c r="L28">
-        <v>74.11042865897905</v>
+        <v>77.449117209254</v>
       </c>
     </row>
     <row r="29" spans="4:12">
@@ -1416,28 +1416,28 @@
         <v>40</v>
       </c>
       <c r="E29">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F29">
+        <v>3</v>
+      </c>
+      <c r="G29">
         <v>2</v>
       </c>
-      <c r="G29">
-        <v>3</v>
-      </c>
       <c r="H29">
-        <v>3998</v>
+        <v>3997</v>
       </c>
       <c r="I29">
-        <v>0.05</v>
+        <v>0.075</v>
       </c>
       <c r="J29">
-        <v>99.95</v>
+        <v>99.925</v>
       </c>
       <c r="K29">
-        <v>96.25</v>
+        <v>97.5</v>
       </c>
       <c r="L29">
-        <v>93.56127385404265</v>
+        <v>94.05125144751109</v>
       </c>
     </row>
     <row r="30" spans="4:12">
@@ -1445,28 +1445,28 @@
         <v>41</v>
       </c>
       <c r="E30">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F30">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G30">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H30">
-        <v>3993</v>
+        <v>3995</v>
       </c>
       <c r="I30">
-        <v>0.175</v>
+        <v>0.125</v>
       </c>
       <c r="J30">
-        <v>99.825</v>
+        <v>99.875</v>
       </c>
       <c r="K30">
-        <v>85</v>
+        <v>87.5</v>
       </c>
       <c r="L30">
-        <v>87.90644205225</v>
+        <v>89.13783048991817</v>
       </c>
     </row>
     <row r="31" spans="4:12">
@@ -1474,28 +1474,28 @@
         <v>42</v>
       </c>
       <c r="E31">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F31">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G31">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H31">
-        <v>3994</v>
+        <v>3992</v>
       </c>
       <c r="I31">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="J31">
-        <v>99.85000000000001</v>
+        <v>99.8</v>
       </c>
       <c r="K31">
-        <v>95</v>
+        <v>98.75</v>
       </c>
       <c r="L31">
-        <v>92.96673617376446</v>
+        <v>94.62898428720069</v>
       </c>
     </row>
     <row r="32" spans="4:12">
@@ -1506,25 +1506,25 @@
         <v>80</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G32">
         <v>0</v>
       </c>
       <c r="H32">
-        <v>4000</v>
+        <v>3999</v>
       </c>
       <c r="I32">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="J32">
-        <v>100</v>
+        <v>99.97500000000001</v>
       </c>
       <c r="K32">
         <v>100</v>
       </c>
       <c r="L32">
-        <v>95.29820002091688</v>
+        <v>95.19914876521705</v>
       </c>
     </row>
     <row r="33" spans="4:12">
@@ -1532,28 +1532,28 @@
         <v>44</v>
       </c>
       <c r="E33">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F33">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G33">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H33">
-        <v>3989</v>
+        <v>3991</v>
       </c>
       <c r="I33">
-        <v>0.275</v>
+        <v>0.225</v>
       </c>
       <c r="J33">
-        <v>99.72499999999999</v>
+        <v>99.77500000000001</v>
       </c>
       <c r="K33">
-        <v>80</v>
+        <v>83.75</v>
       </c>
       <c r="L33">
-        <v>85.15437651382784</v>
+        <v>87.15018567677834</v>
       </c>
     </row>
     <row r="34" spans="4:12">
@@ -1561,28 +1561,28 @@
         <v>45</v>
       </c>
       <c r="E34">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F34">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G34">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H34">
-        <v>3991</v>
+        <v>3992</v>
       </c>
       <c r="I34">
-        <v>0.225</v>
+        <v>0.2</v>
       </c>
       <c r="J34">
-        <v>99.77500000000001</v>
+        <v>99.8</v>
       </c>
       <c r="K34">
-        <v>92.5</v>
+        <v>95</v>
       </c>
       <c r="L34">
-        <v>91.75336338193179</v>
+        <v>92.87246979977959</v>
       </c>
     </row>
     <row r="35" spans="4:12">
@@ -1590,28 +1590,28 @@
         <v>46</v>
       </c>
       <c r="E35">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F35">
+        <v>4</v>
+      </c>
+      <c r="G35">
         <v>3</v>
       </c>
-      <c r="G35">
-        <v>5</v>
-      </c>
       <c r="H35">
-        <v>3997</v>
+        <v>3996</v>
       </c>
       <c r="I35">
-        <v>0.075</v>
+        <v>0.1</v>
       </c>
       <c r="J35">
-        <v>99.925</v>
+        <v>99.90000000000001</v>
       </c>
       <c r="K35">
-        <v>93.75</v>
+        <v>96.25</v>
       </c>
       <c r="L35">
-        <v>92.36415414218204</v>
+        <v>93.46579854569535</v>
       </c>
     </row>
     <row r="36" spans="4:12">
@@ -1619,28 +1619,28 @@
         <v>47</v>
       </c>
       <c r="E36">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F36">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G36">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H36">
-        <v>3992</v>
+        <v>3989</v>
       </c>
       <c r="I36">
-        <v>0.2</v>
+        <v>0.275</v>
       </c>
       <c r="J36">
-        <v>99.8</v>
+        <v>99.72499999999999</v>
       </c>
       <c r="K36">
-        <v>97.5</v>
+        <v>95</v>
       </c>
       <c r="L36">
-        <v>94.14792720067018</v>
+        <v>92.87246979977959</v>
       </c>
     </row>
     <row r="37" spans="4:12">
@@ -1648,28 +1648,28 @@
         <v>48</v>
       </c>
       <c r="E37">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F37">
+        <v>6</v>
+      </c>
+      <c r="G37">
         <v>9</v>
       </c>
-      <c r="G37">
-        <v>7</v>
-      </c>
       <c r="H37">
-        <v>3991</v>
+        <v>3994</v>
       </c>
       <c r="I37">
-        <v>0.225</v>
+        <v>0.15</v>
       </c>
       <c r="J37">
-        <v>99.77500000000001</v>
+        <v>99.85000000000001</v>
       </c>
       <c r="K37">
-        <v>91.25</v>
+        <v>88.75</v>
       </c>
       <c r="L37">
-        <v>91.13419500644522</v>
+        <v>89.78193243555178</v>
       </c>
     </row>
     <row r="38" spans="4:12">
@@ -1698,7 +1698,7 @@
         <v>92.5</v>
       </c>
       <c r="L38">
-        <v>91.75336338193179</v>
+        <v>91.6615404053139</v>
       </c>
     </row>
     <row r="39" spans="4:12">
@@ -1709,25 +1709,25 @@
         <v>80</v>
       </c>
       <c r="F39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G39">
         <v>0</v>
       </c>
       <c r="H39">
-        <v>3999</v>
+        <v>4000</v>
       </c>
       <c r="I39">
-        <v>0.025</v>
+        <v>0</v>
       </c>
       <c r="J39">
-        <v>99.97500000000001</v>
+        <v>100</v>
       </c>
       <c r="K39">
         <v>100</v>
       </c>
       <c r="L39">
-        <v>95.29820002091688</v>
+        <v>95.19914876521705</v>
       </c>
     </row>
     <row r="40" spans="4:12">
@@ -1735,28 +1735,28 @@
         <v>51</v>
       </c>
       <c r="E40">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F40">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H40">
-        <v>3994</v>
+        <v>3992</v>
       </c>
       <c r="I40">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="J40">
-        <v>99.85000000000001</v>
+        <v>99.8</v>
       </c>
       <c r="K40">
-        <v>97.5</v>
+        <v>98.75</v>
       </c>
       <c r="L40">
-        <v>94.14792720067018</v>
+        <v>94.62898428720069</v>
       </c>
     </row>
     <row r="41" spans="4:12">
@@ -1785,7 +1785,7 @@
         <v>88.75</v>
       </c>
       <c r="L41">
-        <v>89.87002637683901</v>
+        <v>89.78193243555178</v>
       </c>
     </row>
     <row r="42" spans="4:12">
@@ -1793,28 +1793,28 @@
         <v>53</v>
       </c>
       <c r="E42">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F42">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G42">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H42">
-        <v>3990</v>
+        <v>3987</v>
       </c>
       <c r="I42">
-        <v>0.25</v>
+        <v>0.325</v>
       </c>
       <c r="J42">
-        <v>99.75</v>
+        <v>99.675</v>
       </c>
       <c r="K42">
-        <v>95</v>
+        <v>91.25</v>
       </c>
       <c r="L42">
-        <v>92.96673617376446</v>
+        <v>91.04360651290163</v>
       </c>
     </row>
     <row r="43" spans="4:12">
@@ -1822,28 +1822,28 @@
         <v>54</v>
       </c>
       <c r="E43">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F43">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G43">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H43">
-        <v>3987</v>
+        <v>3990</v>
       </c>
       <c r="I43">
-        <v>0.325</v>
+        <v>0.25</v>
       </c>
       <c r="J43">
-        <v>99.675</v>
+        <v>99.75</v>
       </c>
       <c r="K43">
-        <v>86.25</v>
+        <v>85</v>
       </c>
       <c r="L43">
-        <v>88.5702008956077</v>
+        <v>87.8221538076715</v>
       </c>
     </row>
     <row r="44" spans="4:12">
@@ -1854,25 +1854,25 @@
         <v>79</v>
       </c>
       <c r="F44">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G44">
         <v>1</v>
       </c>
       <c r="H44">
-        <v>3995</v>
+        <v>3994</v>
       </c>
       <c r="I44">
-        <v>0.125</v>
+        <v>0.15</v>
       </c>
       <c r="J44">
-        <v>99.875</v>
+        <v>99.85000000000001</v>
       </c>
       <c r="K44">
         <v>98.75</v>
       </c>
       <c r="L44">
-        <v>94.72685201517675</v>
+        <v>94.62898428720069</v>
       </c>
     </row>
     <row r="45" spans="4:12">
@@ -1880,28 +1880,28 @@
         <v>56</v>
       </c>
       <c r="E45">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F45">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G45">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H45">
-        <v>3990</v>
+        <v>3992</v>
       </c>
       <c r="I45">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="J45">
-        <v>99.75</v>
+        <v>99.8</v>
       </c>
       <c r="K45">
-        <v>85</v>
+        <v>83.75</v>
       </c>
       <c r="L45">
-        <v>87.90644205225</v>
+        <v>87.15018567677834</v>
       </c>
     </row>
     <row r="46" spans="4:12">
@@ -1909,28 +1909,28 @@
         <v>57</v>
       </c>
       <c r="E46">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F46">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G46">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H46">
-        <v>3997</v>
+        <v>3995</v>
       </c>
       <c r="I46">
-        <v>0.075</v>
+        <v>0.125</v>
       </c>
       <c r="J46">
-        <v>99.925</v>
+        <v>99.875</v>
       </c>
       <c r="K46">
-        <v>86.25</v>
+        <v>85</v>
       </c>
       <c r="L46">
-        <v>88.5702008956077</v>
+        <v>87.8221538076715</v>
       </c>
     </row>
     <row r="47" spans="4:12">
@@ -1938,13 +1938,13 @@
         <v>58</v>
       </c>
       <c r="E47">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F47">
         <v>0</v>
       </c>
       <c r="G47">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H47">
         <v>4000</v>
@@ -1956,10 +1956,10 @@
         <v>100</v>
       </c>
       <c r="K47">
-        <v>97.5</v>
+        <v>96.25</v>
       </c>
       <c r="L47">
-        <v>94.14792720067018</v>
+        <v>93.46579854569535</v>
       </c>
     </row>
     <row r="48" spans="4:12">
@@ -1967,28 +1967,28 @@
         <v>59</v>
       </c>
       <c r="E48">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F48">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G48">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H48">
-        <v>3998</v>
+        <v>3996</v>
       </c>
       <c r="I48">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="J48">
-        <v>99.95</v>
+        <v>99.90000000000001</v>
       </c>
       <c r="K48">
-        <v>97.5</v>
+        <v>96.25</v>
       </c>
       <c r="L48">
-        <v>94.14792720067018</v>
+        <v>93.46579854569535</v>
       </c>
     </row>
     <row r="49" spans="4:12">
@@ -1996,28 +1996,28 @@
         <v>60</v>
       </c>
       <c r="E49">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F49">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G49">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H49">
-        <v>3990</v>
+        <v>3992</v>
       </c>
       <c r="I49">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="J49">
-        <v>99.75</v>
+        <v>99.8</v>
       </c>
       <c r="K49">
-        <v>91.25</v>
+        <v>90</v>
       </c>
       <c r="L49">
-        <v>91.13419500644522</v>
+        <v>90.41712998290244</v>
       </c>
     </row>
     <row r="50" spans="4:12">
@@ -2025,28 +2025,28 @@
         <v>61</v>
       </c>
       <c r="E50">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G50">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H50">
-        <v>4000</v>
+        <v>3999</v>
       </c>
       <c r="I50">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="J50">
-        <v>100</v>
+        <v>99.97500000000001</v>
       </c>
       <c r="K50">
-        <v>91.25</v>
+        <v>92.5</v>
       </c>
       <c r="L50">
-        <v>91.13419500644522</v>
+        <v>91.6615404053139</v>
       </c>
     </row>
     <row r="51" spans="4:12">
@@ -2054,28 +2054,28 @@
         <v>62</v>
       </c>
       <c r="E51">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F51">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G51">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H51">
-        <v>3994</v>
+        <v>3993</v>
       </c>
       <c r="I51">
-        <v>0.15</v>
+        <v>0.175</v>
       </c>
       <c r="J51">
-        <v>99.85000000000001</v>
+        <v>99.825</v>
       </c>
       <c r="K51">
-        <v>82.5</v>
+        <v>83.75</v>
       </c>
       <c r="L51">
-        <v>86.5502347096278</v>
+        <v>87.15018567677834</v>
       </c>
     </row>
     <row r="52" spans="4:12">
@@ -2083,28 +2083,28 @@
         <v>63</v>
       </c>
       <c r="E52">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="F52">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G52">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H52">
-        <v>3994</v>
+        <v>3995</v>
       </c>
       <c r="I52">
-        <v>0.15</v>
+        <v>0.125</v>
       </c>
       <c r="J52">
-        <v>99.85000000000001</v>
+        <v>99.875</v>
       </c>
       <c r="K52">
-        <v>78.75</v>
+        <v>85</v>
       </c>
       <c r="L52">
-        <v>84.44103094416168</v>
+        <v>87.8221538076715</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new metrics, change metrics name, add new plots
</commit_message>
<xml_diff>
--- a/Statisticki podaci modela.xlsx
+++ b/Statisticki podaci modela.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>Jednostavni pokazatelji</t>
   </si>
@@ -43,16 +43,19 @@
     <t>True Negative</t>
   </si>
   <si>
-    <t>False Positive Rate</t>
-  </si>
-  <si>
-    <t>True Negative Rate</t>
+    <t>False Acceptance Rate</t>
+  </si>
+  <si>
+    <t>False Rejection Rate</t>
   </si>
   <si>
     <t>Opoziv</t>
   </si>
   <si>
-    <t>F-mjera</t>
+    <t>Specifičnost</t>
+  </si>
+  <si>
+    <t>F-Mjera</t>
   </si>
   <si>
     <t>s002</t>
@@ -563,7 +566,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L52"/>
+  <dimension ref="A1:M52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -575,7 +578,7 @@
     <col min="9" max="12" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -603,594 +606,654 @@
       <c r="L1" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>11.24628973007202</v>
+        <v>11.34617185592651</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="F2">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G2">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H2">
-        <v>3985</v>
+        <v>3981</v>
       </c>
       <c r="I2">
-        <v>0.375</v>
+        <v>0.475</v>
       </c>
       <c r="J2">
-        <v>99.625</v>
+        <v>23.75</v>
       </c>
       <c r="K2">
-        <v>73.75</v>
+        <v>78.75</v>
       </c>
       <c r="L2">
-        <v>81.40699538055453</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>99.52499999999999</v>
+      </c>
+      <c r="M2">
+        <v>84.35185123430763</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.07761979103088379</v>
+        <v>0.08076810836791992</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3">
         <v>70</v>
       </c>
       <c r="F3">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G3">
         <v>10</v>
       </c>
       <c r="H3">
-        <v>3990</v>
+        <v>3994</v>
       </c>
       <c r="I3">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="J3">
-        <v>99.75</v>
+        <v>7.5</v>
       </c>
       <c r="K3">
         <v>87.5</v>
       </c>
       <c r="L3">
-        <v>89.13783048991817</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>99.85000000000001</v>
+      </c>
+      <c r="M3">
+        <v>89.12510024853437</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>90.80882352941177</v>
+        <v>90.73529411764706</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E4">
         <v>71</v>
       </c>
       <c r="F4">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G4">
         <v>9</v>
       </c>
       <c r="H4">
-        <v>3987</v>
+        <v>3988</v>
       </c>
       <c r="I4">
-        <v>0.325</v>
+        <v>0.3</v>
       </c>
       <c r="J4">
-        <v>99.675</v>
+        <v>15</v>
       </c>
       <c r="K4">
         <v>88.75</v>
       </c>
       <c r="L4">
-        <v>89.78193243555178</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+        <v>99.7</v>
+      </c>
+      <c r="M4">
+        <v>89.76901756764332</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>90.83814457951738</v>
+        <v>90.81170742925568</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F5">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H5">
-        <v>3991</v>
+        <v>3992</v>
       </c>
       <c r="I5">
-        <v>0.225</v>
+        <v>0.2</v>
       </c>
       <c r="J5">
-        <v>99.77500000000001</v>
+        <v>10</v>
       </c>
       <c r="K5">
-        <v>95</v>
+        <v>92.5</v>
       </c>
       <c r="L5">
-        <v>92.87246979977959</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+        <v>99.8</v>
+      </c>
+      <c r="M5">
+        <v>91.64807916535219</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="D6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E6">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="F6">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G6">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H6">
-        <v>3988</v>
+        <v>3990</v>
       </c>
       <c r="I6">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="J6">
-        <v>99.7</v>
+        <v>12.5</v>
       </c>
       <c r="K6">
-        <v>72.5</v>
+        <v>77.5</v>
       </c>
       <c r="L6">
-        <v>80.63965093969686</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+        <v>99.75</v>
+      </c>
+      <c r="M6">
+        <v>83.62944483497049</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="D7" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E7">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="F7">
+        <v>8</v>
+      </c>
+      <c r="G7">
+        <v>11</v>
+      </c>
+      <c r="H7">
+        <v>3992</v>
+      </c>
+      <c r="I7">
+        <v>0.2</v>
+      </c>
+      <c r="J7">
         <v>10</v>
       </c>
-      <c r="G7">
-        <v>15</v>
-      </c>
-      <c r="H7">
-        <v>3990</v>
-      </c>
-      <c r="I7">
-        <v>0.25</v>
-      </c>
-      <c r="J7">
-        <v>99.75</v>
-      </c>
       <c r="K7">
-        <v>81.25</v>
+        <v>86.25</v>
       </c>
       <c r="L7">
-        <v>85.77696348716697</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+        <v>99.8</v>
+      </c>
+      <c r="M7">
+        <v>88.4720912216748</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="D8" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E8">
         <v>79</v>
       </c>
       <c r="F8">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
       <c r="H8">
-        <v>3993</v>
+        <v>3991</v>
       </c>
       <c r="I8">
-        <v>0.175</v>
+        <v>0.225</v>
       </c>
       <c r="J8">
-        <v>99.825</v>
+        <v>11.25</v>
       </c>
       <c r="K8">
         <v>98.75</v>
       </c>
       <c r="L8">
-        <v>94.62898428720069</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>99.77500000000001</v>
+      </c>
+      <c r="M8">
+        <v>94.61463742075357</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="D9" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E9">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>13</v>
+      </c>
+      <c r="H9">
+        <v>3998</v>
+      </c>
+      <c r="I9">
+        <v>0.05</v>
+      </c>
+      <c r="J9">
+        <v>2.5</v>
+      </c>
+      <c r="K9">
+        <v>83.75</v>
+      </c>
+      <c r="L9">
+        <v>99.95</v>
+      </c>
+      <c r="M9">
+        <v>87.13801679881509</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="D10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10">
+        <v>75</v>
+      </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10">
         <v>5</v>
       </c>
-      <c r="G9">
-        <v>11</v>
-      </c>
-      <c r="H9">
-        <v>3995</v>
-      </c>
-      <c r="I9">
-        <v>0.125</v>
-      </c>
-      <c r="J9">
-        <v>99.875</v>
-      </c>
-      <c r="K9">
-        <v>86.25</v>
-      </c>
-      <c r="L9">
-        <v>88.48463558739631</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="D10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10">
-        <v>74</v>
-      </c>
-      <c r="F10">
-        <v>4</v>
-      </c>
-      <c r="G10">
-        <v>6</v>
-      </c>
       <c r="H10">
-        <v>3996</v>
+        <v>3992</v>
       </c>
       <c r="I10">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="J10">
-        <v>99.90000000000001</v>
+        <v>10</v>
       </c>
       <c r="K10">
-        <v>92.5</v>
+        <v>93.75</v>
       </c>
       <c r="L10">
-        <v>91.6615404053139</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>99.8</v>
+      </c>
+      <c r="M10">
+        <v>92.25746434705114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="D11" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E11">
         <v>72</v>
       </c>
       <c r="F11">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G11">
         <v>8</v>
       </c>
       <c r="H11">
-        <v>3986</v>
+        <v>3995</v>
       </c>
       <c r="I11">
-        <v>0.35</v>
+        <v>0.125</v>
       </c>
       <c r="J11">
-        <v>99.65000000000001</v>
+        <v>6.25</v>
       </c>
       <c r="K11">
         <v>90</v>
       </c>
       <c r="L11">
-        <v>90.41712998290244</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>99.875</v>
+      </c>
+      <c r="M11">
+        <v>90.40403173926994</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="D12" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E12">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="F12">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G12">
+        <v>11</v>
+      </c>
+      <c r="H12">
+        <v>3988</v>
+      </c>
+      <c r="I12">
+        <v>0.3</v>
+      </c>
+      <c r="J12">
         <v>15</v>
       </c>
-      <c r="H12">
-        <v>3991</v>
-      </c>
-      <c r="I12">
-        <v>0.225</v>
-      </c>
-      <c r="J12">
-        <v>99.77500000000001</v>
-      </c>
       <c r="K12">
-        <v>81.25</v>
+        <v>86.25</v>
       </c>
       <c r="L12">
-        <v>85.77696348716697</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+        <v>99.7</v>
+      </c>
+      <c r="M12">
+        <v>88.4720912216748</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="D13" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E13">
+        <v>77</v>
+      </c>
+      <c r="F13">
+        <v>13</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <v>3987</v>
+      </c>
+      <c r="I13">
+        <v>0.325</v>
+      </c>
+      <c r="J13">
+        <v>16.25</v>
+      </c>
+      <c r="K13">
+        <v>96.25</v>
+      </c>
+      <c r="L13">
+        <v>99.675</v>
+      </c>
+      <c r="M13">
+        <v>93.45180219069103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="D14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14">
         <v>79</v>
       </c>
-      <c r="F13">
-        <v>15</v>
-      </c>
-      <c r="G13">
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
         <v>1</v>
       </c>
-      <c r="H13">
-        <v>3985</v>
-      </c>
-      <c r="I13">
-        <v>0.375</v>
-      </c>
-      <c r="J13">
-        <v>99.625</v>
-      </c>
-      <c r="K13">
+      <c r="H14">
+        <v>4000</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
         <v>98.75</v>
       </c>
-      <c r="L13">
-        <v>94.62898428720069</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="D14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14">
-        <v>77</v>
-      </c>
-      <c r="F14">
-        <v>4</v>
-      </c>
-      <c r="G14">
-        <v>3</v>
-      </c>
-      <c r="H14">
-        <v>3996</v>
-      </c>
-      <c r="I14">
-        <v>0.1</v>
-      </c>
-      <c r="J14">
-        <v>99.90000000000001</v>
-      </c>
-      <c r="K14">
-        <v>96.25</v>
-      </c>
       <c r="L14">
-        <v>93.46579854569535</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>100</v>
+      </c>
+      <c r="M14">
+        <v>94.61463742075357</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="D15" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E15">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F15">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G15">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H15">
-        <v>3991</v>
+        <v>3989</v>
       </c>
       <c r="I15">
-        <v>0.225</v>
+        <v>0.275</v>
       </c>
       <c r="J15">
-        <v>99.77500000000001</v>
+        <v>13.75</v>
       </c>
       <c r="K15">
-        <v>82.5</v>
+        <v>86.25</v>
       </c>
       <c r="L15">
-        <v>86.46852596685443</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+        <v>99.72499999999999</v>
+      </c>
+      <c r="M15">
+        <v>88.4720912216748</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="D16" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E16">
         <v>79</v>
       </c>
       <c r="F16">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G16">
         <v>1</v>
       </c>
       <c r="H16">
-        <v>3995</v>
+        <v>3993</v>
       </c>
       <c r="I16">
-        <v>0.125</v>
+        <v>0.175</v>
       </c>
       <c r="J16">
-        <v>99.875</v>
+        <v>8.75</v>
       </c>
       <c r="K16">
         <v>98.75</v>
       </c>
       <c r="L16">
-        <v>94.62898428720069</v>
-      </c>
-    </row>
-    <row r="17" spans="4:12">
+        <v>99.825</v>
+      </c>
+      <c r="M16">
+        <v>94.61463742075357</v>
+      </c>
+    </row>
+    <row r="17" spans="4:13">
       <c r="D17" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E17">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F17">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G17">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H17">
-        <v>3993</v>
+        <v>3995</v>
       </c>
       <c r="I17">
-        <v>0.175</v>
+        <v>0.125</v>
       </c>
       <c r="J17">
-        <v>99.825</v>
+        <v>6.25</v>
       </c>
       <c r="K17">
-        <v>78.75</v>
+        <v>81.25</v>
       </c>
       <c r="L17">
-        <v>84.36325432268436</v>
-      </c>
-    </row>
-    <row r="18" spans="4:12">
+        <v>99.875</v>
+      </c>
+      <c r="M17">
+        <v>85.76517505105805</v>
+      </c>
+    </row>
+    <row r="18" spans="4:13">
       <c r="D18" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E18">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F18">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="G18">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H18">
-        <v>3993</v>
+        <v>3984</v>
       </c>
       <c r="I18">
-        <v>0.175</v>
+        <v>0.4</v>
       </c>
       <c r="J18">
-        <v>99.825</v>
+        <v>20</v>
       </c>
       <c r="K18">
-        <v>92.5</v>
+        <v>93.75</v>
       </c>
       <c r="L18">
-        <v>91.6615404053139</v>
-      </c>
-    </row>
-    <row r="19" spans="4:12">
+        <v>99.59999999999999</v>
+      </c>
+      <c r="M18">
+        <v>92.25746434705114</v>
+      </c>
+    </row>
+    <row r="19" spans="4:13">
       <c r="D19" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E19">
         <v>80</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19">
-        <v>3999</v>
+        <v>4000</v>
       </c>
       <c r="I19">
-        <v>0.025</v>
+        <v>0</v>
       </c>
       <c r="J19">
-        <v>99.97500000000001</v>
+        <v>0</v>
       </c>
       <c r="K19">
         <v>100</v>
       </c>
       <c r="L19">
-        <v>95.19914876521705</v>
-      </c>
-    </row>
-    <row r="20" spans="4:12">
+        <v>100</v>
+      </c>
+      <c r="M19">
+        <v>95.18462850391352</v>
+      </c>
+    </row>
+    <row r="20" spans="4:13">
       <c r="D20" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E20">
         <v>80</v>
       </c>
       <c r="F20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
       <c r="H20">
-        <v>3997</v>
+        <v>3996</v>
       </c>
       <c r="I20">
-        <v>0.075</v>
+        <v>0.1</v>
       </c>
       <c r="J20">
-        <v>99.925</v>
+        <v>5</v>
       </c>
       <c r="K20">
         <v>100</v>
       </c>
       <c r="L20">
-        <v>95.19914876521705</v>
-      </c>
-    </row>
-    <row r="21" spans="4:12">
+        <v>99.90000000000001</v>
+      </c>
+      <c r="M20">
+        <v>95.18462850391352</v>
+      </c>
+    </row>
+    <row r="21" spans="4:13">
       <c r="D21" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E21">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F21">
         <v>8</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H21">
         <v>3992</v>
@@ -1199,114 +1262,126 @@
         <v>0.2</v>
       </c>
       <c r="J21">
+        <v>10</v>
+      </c>
+      <c r="K21">
+        <v>97.5</v>
+      </c>
+      <c r="L21">
         <v>99.8</v>
       </c>
-      <c r="K21">
-        <v>100</v>
-      </c>
-      <c r="L21">
-        <v>95.19914876521705</v>
-      </c>
-    </row>
-    <row r="22" spans="4:12">
+      <c r="M21">
+        <v>94.0370792153613</v>
+      </c>
+    </row>
+    <row r="22" spans="4:13">
       <c r="D22" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E22">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F22">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G22">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H22">
-        <v>3991</v>
+        <v>3989</v>
       </c>
       <c r="I22">
-        <v>0.225</v>
+        <v>0.275</v>
       </c>
       <c r="J22">
-        <v>99.77500000000001</v>
+        <v>13.75</v>
       </c>
       <c r="K22">
-        <v>93.75</v>
+        <v>90</v>
       </c>
       <c r="L22">
-        <v>92.2711052080723</v>
-      </c>
-    </row>
-    <row r="23" spans="4:12">
+        <v>99.72499999999999</v>
+      </c>
+      <c r="M22">
+        <v>90.40403173926994</v>
+      </c>
+    </row>
+    <row r="23" spans="4:13">
       <c r="D23" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E23">
         <v>78</v>
       </c>
       <c r="F23">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G23">
         <v>2</v>
       </c>
       <c r="H23">
-        <v>3995</v>
+        <v>3992</v>
       </c>
       <c r="I23">
-        <v>0.125</v>
+        <v>0.2</v>
       </c>
       <c r="J23">
-        <v>99.875</v>
+        <v>10</v>
       </c>
       <c r="K23">
         <v>97.5</v>
       </c>
       <c r="L23">
-        <v>94.05125144751109</v>
-      </c>
-    </row>
-    <row r="24" spans="4:12">
+        <v>99.8</v>
+      </c>
+      <c r="M23">
+        <v>94.0370792153613</v>
+      </c>
+    </row>
+    <row r="24" spans="4:13">
       <c r="D24" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E24">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H24">
-        <v>4000</v>
+        <v>3999</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="J24">
-        <v>100</v>
+        <v>1.25</v>
       </c>
       <c r="K24">
-        <v>97.5</v>
+        <v>98.75</v>
       </c>
       <c r="L24">
-        <v>94.05125144751109</v>
-      </c>
-    </row>
-    <row r="25" spans="4:12">
+        <v>99.97500000000001</v>
+      </c>
+      <c r="M24">
+        <v>94.61463742075357</v>
+      </c>
+    </row>
+    <row r="25" spans="4:13">
       <c r="D25" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E25">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F25">
         <v>10</v>
       </c>
       <c r="G25">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H25">
         <v>3990</v>
@@ -1315,192 +1390,213 @@
         <v>0.25</v>
       </c>
       <c r="J25">
+        <v>12.5</v>
+      </c>
+      <c r="K25">
+        <v>85</v>
+      </c>
+      <c r="L25">
         <v>99.75</v>
       </c>
-      <c r="K25">
-        <v>87.5</v>
-      </c>
-      <c r="L25">
-        <v>89.13783048991817</v>
-      </c>
-    </row>
-    <row r="26" spans="4:12">
+      <c r="M25">
+        <v>87.80979656423341</v>
+      </c>
+    </row>
+    <row r="26" spans="4:13">
       <c r="D26" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E26">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F26">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G26">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H26">
-        <v>3994</v>
+        <v>3995</v>
       </c>
       <c r="I26">
-        <v>0.15</v>
+        <v>0.125</v>
       </c>
       <c r="J26">
-        <v>99.85000000000001</v>
+        <v>6.25</v>
       </c>
       <c r="K26">
-        <v>98.75</v>
+        <v>93.75</v>
       </c>
       <c r="L26">
-        <v>94.62898428720069</v>
-      </c>
-    </row>
-    <row r="27" spans="4:12">
+        <v>99.875</v>
+      </c>
+      <c r="M26">
+        <v>92.25746434705114</v>
+      </c>
+    </row>
+    <row r="27" spans="4:13">
       <c r="D27" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E27">
         <v>67</v>
       </c>
       <c r="F27">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G27">
         <v>13</v>
       </c>
       <c r="H27">
-        <v>3977</v>
+        <v>3979</v>
       </c>
       <c r="I27">
-        <v>0.575</v>
+        <v>0.525</v>
       </c>
       <c r="J27">
-        <v>99.425</v>
+        <v>26.25</v>
       </c>
       <c r="K27">
         <v>83.75</v>
       </c>
       <c r="L27">
-        <v>87.15018567677834</v>
-      </c>
-    </row>
-    <row r="28" spans="4:12">
+        <v>99.47500000000001</v>
+      </c>
+      <c r="M27">
+        <v>87.13801679881509</v>
+      </c>
+    </row>
+    <row r="28" spans="4:13">
       <c r="D28" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E28">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F28">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G28">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="H28">
-        <v>3983</v>
+        <v>3985</v>
       </c>
       <c r="I28">
-        <v>0.425</v>
+        <v>0.375</v>
       </c>
       <c r="J28">
-        <v>99.575</v>
+        <v>18.75</v>
       </c>
       <c r="K28">
-        <v>67.5</v>
+        <v>58.75</v>
       </c>
       <c r="L28">
-        <v>77.449117209254</v>
-      </c>
-    </row>
-    <row r="29" spans="4:12">
+        <v>99.625</v>
+      </c>
+      <c r="M28">
+        <v>71.34430200313636</v>
+      </c>
+    </row>
+    <row r="29" spans="4:13">
       <c r="D29" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E29">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H29">
-        <v>3997</v>
+        <v>3998</v>
       </c>
       <c r="I29">
-        <v>0.075</v>
+        <v>0.05</v>
       </c>
       <c r="J29">
-        <v>99.925</v>
+        <v>2.5</v>
       </c>
       <c r="K29">
-        <v>97.5</v>
+        <v>98.75</v>
       </c>
       <c r="L29">
-        <v>94.05125144751109</v>
-      </c>
-    </row>
-    <row r="30" spans="4:12">
+        <v>99.95</v>
+      </c>
+      <c r="M29">
+        <v>94.61463742075357</v>
+      </c>
+    </row>
+    <row r="30" spans="4:13">
       <c r="D30" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E30">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F30">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G30">
+        <v>7</v>
+      </c>
+      <c r="H30">
+        <v>3992</v>
+      </c>
+      <c r="I30">
+        <v>0.2</v>
+      </c>
+      <c r="J30">
         <v>10</v>
       </c>
-      <c r="H30">
-        <v>3995</v>
-      </c>
-      <c r="I30">
-        <v>0.125</v>
-      </c>
-      <c r="J30">
-        <v>99.875</v>
-      </c>
       <c r="K30">
-        <v>87.5</v>
+        <v>91.25</v>
       </c>
       <c r="L30">
-        <v>89.13783048991817</v>
-      </c>
-    </row>
-    <row r="31" spans="4:12">
+        <v>99.8</v>
+      </c>
+      <c r="M30">
+        <v>91.03032614521118</v>
+      </c>
+    </row>
+    <row r="31" spans="4:13">
       <c r="D31" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E31">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F31">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G31">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H31">
-        <v>3992</v>
+        <v>3991</v>
       </c>
       <c r="I31">
-        <v>0.2</v>
+        <v>0.225</v>
       </c>
       <c r="J31">
-        <v>99.8</v>
+        <v>11.25</v>
       </c>
       <c r="K31">
-        <v>98.75</v>
+        <v>95</v>
       </c>
       <c r="L31">
-        <v>94.62898428720069</v>
-      </c>
-    </row>
-    <row r="32" spans="4:12">
+        <v>99.77500000000001</v>
+      </c>
+      <c r="M31">
+        <v>92.85865056768719</v>
+      </c>
+    </row>
+    <row r="32" spans="4:13">
       <c r="D32" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E32">
         <v>80</v>
@@ -1518,56 +1614,62 @@
         <v>0.025</v>
       </c>
       <c r="J32">
-        <v>99.97500000000001</v>
+        <v>1.25</v>
       </c>
       <c r="K32">
         <v>100</v>
       </c>
       <c r="L32">
-        <v>95.19914876521705</v>
-      </c>
-    </row>
-    <row r="33" spans="4:12">
+        <v>99.97500000000001</v>
+      </c>
+      <c r="M32">
+        <v>95.18462850391352</v>
+      </c>
+    </row>
+    <row r="33" spans="4:13">
       <c r="D33" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E33">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F33">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G33">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H33">
-        <v>3991</v>
+        <v>3992</v>
       </c>
       <c r="I33">
-        <v>0.225</v>
+        <v>0.2</v>
       </c>
       <c r="J33">
-        <v>99.77500000000001</v>
+        <v>10</v>
       </c>
       <c r="K33">
-        <v>83.75</v>
+        <v>81.25</v>
       </c>
       <c r="L33">
-        <v>87.15018567677834</v>
-      </c>
-    </row>
-    <row r="34" spans="4:12">
+        <v>99.8</v>
+      </c>
+      <c r="M33">
+        <v>85.76517505105805</v>
+      </c>
+    </row>
+    <row r="34" spans="4:13">
       <c r="D34" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E34">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F34">
         <v>8</v>
       </c>
       <c r="G34">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H34">
         <v>3992</v>
@@ -1576,56 +1678,62 @@
         <v>0.2</v>
       </c>
       <c r="J34">
+        <v>10</v>
+      </c>
+      <c r="K34">
+        <v>96.25</v>
+      </c>
+      <c r="L34">
         <v>99.8</v>
       </c>
-      <c r="K34">
-        <v>95</v>
-      </c>
-      <c r="L34">
-        <v>92.87246979977959</v>
-      </c>
-    </row>
-    <row r="35" spans="4:12">
+      <c r="M34">
+        <v>93.45180219069103</v>
+      </c>
+    </row>
+    <row r="35" spans="4:13">
       <c r="D35" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E35">
+        <v>74</v>
+      </c>
+      <c r="F35">
+        <v>6</v>
+      </c>
+      <c r="G35">
+        <v>6</v>
+      </c>
+      <c r="H35">
+        <v>3994</v>
+      </c>
+      <c r="I35">
+        <v>0.15</v>
+      </c>
+      <c r="J35">
+        <v>7.5</v>
+      </c>
+      <c r="K35">
+        <v>92.5</v>
+      </c>
+      <c r="L35">
+        <v>99.85000000000001</v>
+      </c>
+      <c r="M35">
+        <v>91.64807916535219</v>
+      </c>
+    </row>
+    <row r="36" spans="4:13">
+      <c r="D36" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E36">
         <v>77</v>
-      </c>
-      <c r="F35">
-        <v>4</v>
-      </c>
-      <c r="G35">
-        <v>3</v>
-      </c>
-      <c r="H35">
-        <v>3996</v>
-      </c>
-      <c r="I35">
-        <v>0.1</v>
-      </c>
-      <c r="J35">
-        <v>99.90000000000001</v>
-      </c>
-      <c r="K35">
-        <v>96.25</v>
-      </c>
-      <c r="L35">
-        <v>93.46579854569535</v>
-      </c>
-    </row>
-    <row r="36" spans="4:12">
-      <c r="D36" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E36">
-        <v>76</v>
       </c>
       <c r="F36">
         <v>11</v>
       </c>
       <c r="G36">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H36">
         <v>3989</v>
@@ -1634,172 +1742,190 @@
         <v>0.275</v>
       </c>
       <c r="J36">
+        <v>13.75</v>
+      </c>
+      <c r="K36">
+        <v>96.25</v>
+      </c>
+      <c r="L36">
         <v>99.72499999999999</v>
       </c>
-      <c r="K36">
-        <v>95</v>
-      </c>
-      <c r="L36">
-        <v>92.87246979977959</v>
-      </c>
-    </row>
-    <row r="37" spans="4:12">
+      <c r="M36">
+        <v>93.45180219069103</v>
+      </c>
+    </row>
+    <row r="37" spans="4:13">
       <c r="D37" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E37">
         <v>71</v>
       </c>
       <c r="F37">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G37">
         <v>9</v>
       </c>
       <c r="H37">
-        <v>3994</v>
+        <v>3991</v>
       </c>
       <c r="I37">
-        <v>0.15</v>
+        <v>0.225</v>
       </c>
       <c r="J37">
-        <v>99.85000000000001</v>
+        <v>11.25</v>
       </c>
       <c r="K37">
         <v>88.75</v>
       </c>
       <c r="L37">
-        <v>89.78193243555178</v>
-      </c>
-    </row>
-    <row r="38" spans="4:12">
+        <v>99.77500000000001</v>
+      </c>
+      <c r="M37">
+        <v>89.76901756764332</v>
+      </c>
+    </row>
+    <row r="38" spans="4:13">
       <c r="D38" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E38">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G38">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H38">
-        <v>3998</v>
+        <v>3999</v>
       </c>
       <c r="I38">
-        <v>0.05</v>
+        <v>0.025</v>
       </c>
       <c r="J38">
-        <v>99.95</v>
+        <v>1.25</v>
       </c>
       <c r="K38">
-        <v>92.5</v>
+        <v>93.75</v>
       </c>
       <c r="L38">
-        <v>91.6615404053139</v>
-      </c>
-    </row>
-    <row r="39" spans="4:12">
+        <v>99.97500000000001</v>
+      </c>
+      <c r="M38">
+        <v>92.25746434705114</v>
+      </c>
+    </row>
+    <row r="39" spans="4:13">
       <c r="D39" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E39">
         <v>80</v>
       </c>
       <c r="F39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G39">
         <v>0</v>
       </c>
       <c r="H39">
-        <v>4000</v>
+        <v>3999</v>
       </c>
       <c r="I39">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="J39">
-        <v>100</v>
+        <v>1.25</v>
       </c>
       <c r="K39">
         <v>100</v>
       </c>
       <c r="L39">
-        <v>95.19914876521705</v>
-      </c>
-    </row>
-    <row r="40" spans="4:12">
+        <v>99.97500000000001</v>
+      </c>
+      <c r="M39">
+        <v>95.18462850391352</v>
+      </c>
+    </row>
+    <row r="40" spans="4:13">
       <c r="D40" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E40">
         <v>79</v>
       </c>
       <c r="F40">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G40">
         <v>1</v>
       </c>
       <c r="H40">
-        <v>3992</v>
+        <v>3995</v>
       </c>
       <c r="I40">
-        <v>0.2</v>
+        <v>0.125</v>
       </c>
       <c r="J40">
-        <v>99.8</v>
+        <v>6.25</v>
       </c>
       <c r="K40">
         <v>98.75</v>
       </c>
       <c r="L40">
-        <v>94.62898428720069</v>
-      </c>
-    </row>
-    <row r="41" spans="4:12">
+        <v>99.875</v>
+      </c>
+      <c r="M40">
+        <v>94.61463742075357</v>
+      </c>
+    </row>
+    <row r="41" spans="4:13">
       <c r="D41" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E41">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F41">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G41">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H41">
-        <v>3994</v>
+        <v>3988</v>
       </c>
       <c r="I41">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
       <c r="J41">
-        <v>99.85000000000001</v>
+        <v>15</v>
       </c>
       <c r="K41">
-        <v>88.75</v>
+        <v>86.25</v>
       </c>
       <c r="L41">
-        <v>89.78193243555178</v>
-      </c>
-    </row>
-    <row r="42" spans="4:12">
+        <v>99.7</v>
+      </c>
+      <c r="M41">
+        <v>88.4720912216748</v>
+      </c>
+    </row>
+    <row r="42" spans="4:13">
       <c r="D42" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E42">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F42">
         <v>13</v>
       </c>
       <c r="G42">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H42">
         <v>3987</v>
@@ -1808,76 +1934,85 @@
         <v>0.325</v>
       </c>
       <c r="J42">
+        <v>16.25</v>
+      </c>
+      <c r="K42">
+        <v>95</v>
+      </c>
+      <c r="L42">
         <v>99.675</v>
       </c>
-      <c r="K42">
-        <v>91.25</v>
-      </c>
-      <c r="L42">
-        <v>91.04360651290163</v>
-      </c>
-    </row>
-    <row r="43" spans="4:12">
+      <c r="M42">
+        <v>92.85865056768719</v>
+      </c>
+    </row>
+    <row r="43" spans="4:13">
       <c r="D43" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E43">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F43">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G43">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H43">
-        <v>3990</v>
+        <v>3989</v>
       </c>
       <c r="I43">
-        <v>0.25</v>
+        <v>0.275</v>
       </c>
       <c r="J43">
-        <v>99.75</v>
+        <v>13.75</v>
       </c>
       <c r="K43">
-        <v>85</v>
+        <v>83.75</v>
       </c>
       <c r="L43">
-        <v>87.8221538076715</v>
-      </c>
-    </row>
-    <row r="44" spans="4:12">
+        <v>99.72499999999999</v>
+      </c>
+      <c r="M43">
+        <v>87.13801679881509</v>
+      </c>
+    </row>
+    <row r="44" spans="4:13">
       <c r="D44" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E44">
         <v>79</v>
       </c>
       <c r="F44">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G44">
         <v>1</v>
       </c>
       <c r="H44">
-        <v>3994</v>
+        <v>3996</v>
       </c>
       <c r="I44">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="J44">
-        <v>99.85000000000001</v>
+        <v>5</v>
       </c>
       <c r="K44">
         <v>98.75</v>
       </c>
       <c r="L44">
-        <v>94.62898428720069</v>
-      </c>
-    </row>
-    <row r="45" spans="4:12">
+        <v>99.90000000000001</v>
+      </c>
+      <c r="M44">
+        <v>94.61463742075357</v>
+      </c>
+    </row>
+    <row r="45" spans="4:13">
       <c r="D45" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E45">
         <v>67</v>
@@ -1895,56 +2030,62 @@
         <v>0.2</v>
       </c>
       <c r="J45">
-        <v>99.8</v>
+        <v>10</v>
       </c>
       <c r="K45">
         <v>83.75</v>
       </c>
       <c r="L45">
-        <v>87.15018567677834</v>
-      </c>
-    </row>
-    <row r="46" spans="4:12">
+        <v>99.8</v>
+      </c>
+      <c r="M45">
+        <v>87.13801679881509</v>
+      </c>
+    </row>
+    <row r="46" spans="4:13">
       <c r="D46" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E46">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F46">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G46">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H46">
-        <v>3995</v>
+        <v>3997</v>
       </c>
       <c r="I46">
-        <v>0.125</v>
+        <v>0.075</v>
       </c>
       <c r="J46">
-        <v>99.875</v>
+        <v>3.75</v>
       </c>
       <c r="K46">
-        <v>85</v>
+        <v>81.25</v>
       </c>
       <c r="L46">
-        <v>87.8221538076715</v>
-      </c>
-    </row>
-    <row r="47" spans="4:12">
+        <v>99.925</v>
+      </c>
+      <c r="M46">
+        <v>85.76517505105805</v>
+      </c>
+    </row>
+    <row r="47" spans="4:13">
       <c r="D47" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E47">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F47">
         <v>0</v>
       </c>
       <c r="G47">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H47">
         <v>4000</v>
@@ -1953,114 +2094,126 @@
         <v>0</v>
       </c>
       <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>97.5</v>
+      </c>
+      <c r="L47">
         <v>100</v>
       </c>
-      <c r="K47">
-        <v>96.25</v>
-      </c>
-      <c r="L47">
-        <v>93.46579854569535</v>
-      </c>
-    </row>
-    <row r="48" spans="4:12">
+      <c r="M47">
+        <v>94.0370792153613</v>
+      </c>
+    </row>
+    <row r="48" spans="4:13">
       <c r="D48" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E48">
         <v>77</v>
       </c>
       <c r="F48">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G48">
         <v>3</v>
       </c>
       <c r="H48">
-        <v>3996</v>
+        <v>4000</v>
       </c>
       <c r="I48">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="J48">
-        <v>99.90000000000001</v>
+        <v>0</v>
       </c>
       <c r="K48">
         <v>96.25</v>
       </c>
       <c r="L48">
-        <v>93.46579854569535</v>
-      </c>
-    </row>
-    <row r="49" spans="4:12">
+        <v>100</v>
+      </c>
+      <c r="M48">
+        <v>93.45180219069103</v>
+      </c>
+    </row>
+    <row r="49" spans="4:13">
       <c r="D49" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E49">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F49">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G49">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H49">
-        <v>3992</v>
+        <v>3990</v>
       </c>
       <c r="I49">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="J49">
-        <v>99.8</v>
+        <v>12.5</v>
       </c>
       <c r="K49">
-        <v>90</v>
+        <v>86.25</v>
       </c>
       <c r="L49">
-        <v>90.41712998290244</v>
-      </c>
-    </row>
-    <row r="50" spans="4:12">
+        <v>99.75</v>
+      </c>
+      <c r="M49">
+        <v>88.4720912216748</v>
+      </c>
+    </row>
+    <row r="50" spans="4:13">
       <c r="D50" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E50">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G50">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H50">
-        <v>3999</v>
+        <v>4000</v>
       </c>
       <c r="I50">
-        <v>0.025</v>
+        <v>0</v>
       </c>
       <c r="J50">
-        <v>99.97500000000001</v>
+        <v>0</v>
       </c>
       <c r="K50">
-        <v>92.5</v>
+        <v>91.25</v>
       </c>
       <c r="L50">
-        <v>91.6615404053139</v>
-      </c>
-    </row>
-    <row r="51" spans="4:12">
+        <v>100</v>
+      </c>
+      <c r="M50">
+        <v>91.03032614521118</v>
+      </c>
+    </row>
+    <row r="51" spans="4:13">
       <c r="D51" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E51">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F51">
         <v>7</v>
       </c>
       <c r="G51">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H51">
         <v>3993</v>
@@ -2069,42 +2222,48 @@
         <v>0.175</v>
       </c>
       <c r="J51">
+        <v>8.75</v>
+      </c>
+      <c r="K51">
+        <v>86.25</v>
+      </c>
+      <c r="L51">
         <v>99.825</v>
       </c>
-      <c r="K51">
-        <v>83.75</v>
-      </c>
-      <c r="L51">
-        <v>87.15018567677834</v>
-      </c>
-    </row>
-    <row r="52" spans="4:12">
+      <c r="M51">
+        <v>88.4720912216748</v>
+      </c>
+    </row>
+    <row r="52" spans="4:13">
       <c r="D52" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E52">
         <v>68</v>
       </c>
       <c r="F52">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G52">
         <v>12</v>
       </c>
       <c r="H52">
-        <v>3995</v>
+        <v>3993</v>
       </c>
       <c r="I52">
-        <v>0.125</v>
+        <v>0.175</v>
       </c>
       <c r="J52">
-        <v>99.875</v>
+        <v>8.75</v>
       </c>
       <c r="K52">
         <v>85</v>
       </c>
       <c r="L52">
-        <v>87.8221538076715</v>
+        <v>99.825</v>
+      </c>
+      <c r="M52">
+        <v>87.80979656423341</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add pictures, change titles
</commit_message>
<xml_diff>
--- a/Statisticki podaci modela.xlsx
+++ b/Statisticki podaci modela.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
-    <t>Jednostavni pokazatelji</t>
+    <t>Iznos</t>
   </si>
   <si>
     <t>Vrijeme treniranja</t>
@@ -43,10 +43,10 @@
     <t>True Negative</t>
   </si>
   <si>
-    <t>False Acceptance Rate</t>
-  </si>
-  <si>
-    <t>False Rejection Rate</t>
+    <t>Stopa pogrešnog prihvaćanja</t>
+  </si>
+  <si>
+    <t>Stopa pogrešnog  odbijanja</t>
   </si>
   <si>
     <t>Opoziv</t>
@@ -615,37 +615,37 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>11.08382701873779</v>
+        <v>11.46561646461487</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E2">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F2">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H2">
-        <v>3980</v>
+        <v>3983</v>
       </c>
       <c r="I2">
-        <v>0.5</v>
+        <v>0.425</v>
       </c>
       <c r="J2">
-        <v>25</v>
+        <v>21.25</v>
       </c>
       <c r="K2">
-        <v>78.75</v>
+        <v>77.5</v>
       </c>
       <c r="L2">
-        <v>99.5</v>
+        <v>99.575</v>
       </c>
       <c r="M2">
-        <v>84.5008279409199</v>
+        <v>83.68930020654656</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -653,37 +653,37 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.07289385795593262</v>
+        <v>0.07068371772766113</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E3">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G3">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H3">
-        <v>3990</v>
+        <v>3989</v>
       </c>
       <c r="I3">
-        <v>0.25</v>
+        <v>0.275</v>
       </c>
       <c r="J3">
-        <v>12.5</v>
+        <v>13.75</v>
       </c>
       <c r="K3">
-        <v>87.5</v>
+        <v>91.25</v>
       </c>
       <c r="L3">
-        <v>99.75</v>
+        <v>99.72499999999999</v>
       </c>
       <c r="M3">
-        <v>89.29143101977752</v>
+        <v>91.10124870622212</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -691,7 +691,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>90.98039215686275</v>
+        <v>90.83333333333333</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>16</v>
@@ -700,28 +700,28 @@
         <v>72</v>
       </c>
       <c r="F4">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G4">
         <v>8</v>
       </c>
       <c r="H4">
-        <v>3984</v>
+        <v>3986</v>
       </c>
       <c r="I4">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="J4">
-        <v>20</v>
+        <v>17.5</v>
       </c>
       <c r="K4">
         <v>90</v>
       </c>
       <c r="L4">
-        <v>99.59999999999999</v>
+        <v>99.65000000000001</v>
       </c>
       <c r="M4">
-        <v>90.57517498634861</v>
+        <v>90.47398137904899</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -729,7 +729,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>91.15774895312285</v>
+        <v>90.95298159733929</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>17</v>
@@ -738,28 +738,28 @@
         <v>77</v>
       </c>
       <c r="F5">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G5">
         <v>3</v>
       </c>
       <c r="H5">
-        <v>3995</v>
+        <v>3992</v>
       </c>
       <c r="I5">
-        <v>0.125</v>
+        <v>0.2</v>
       </c>
       <c r="J5">
-        <v>6.25</v>
+        <v>10</v>
       </c>
       <c r="K5">
         <v>96.25</v>
       </c>
       <c r="L5">
-        <v>99.875</v>
+        <v>99.8</v>
       </c>
       <c r="M5">
-        <v>93.6346910493305</v>
+        <v>93.52654967401791</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -767,31 +767,31 @@
         <v>18</v>
       </c>
       <c r="E6">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F6">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G6">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H6">
-        <v>3987</v>
+        <v>3988</v>
       </c>
       <c r="I6">
-        <v>0.325</v>
+        <v>0.3</v>
       </c>
       <c r="J6">
-        <v>16.25</v>
+        <v>15</v>
       </c>
       <c r="K6">
-        <v>77.5</v>
+        <v>80</v>
       </c>
       <c r="L6">
-        <v>99.675</v>
+        <v>99.7</v>
       </c>
       <c r="M6">
-        <v>83.77587851988477</v>
+        <v>85.12561126223014</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -799,31 +799,31 @@
         <v>19</v>
       </c>
       <c r="E7">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="F7">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G7">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="H7">
-        <v>3994</v>
+        <v>3989</v>
       </c>
       <c r="I7">
-        <v>0.15</v>
+        <v>0.275</v>
       </c>
       <c r="J7">
-        <v>7.5</v>
+        <v>13.75</v>
       </c>
       <c r="K7">
-        <v>83.75</v>
+        <v>90</v>
       </c>
       <c r="L7">
-        <v>99.85000000000001</v>
+        <v>99.72499999999999</v>
       </c>
       <c r="M7">
-        <v>87.29700679951185</v>
+        <v>90.47398137904899</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -831,13 +831,13 @@
         <v>20</v>
       </c>
       <c r="E8">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F8">
         <v>6</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H8">
         <v>3994</v>
@@ -849,13 +849,13 @@
         <v>7.5</v>
       </c>
       <c r="K8">
-        <v>100</v>
+        <v>96.25</v>
       </c>
       <c r="L8">
         <v>99.85000000000001</v>
       </c>
       <c r="M8">
-        <v>95.37436954802941</v>
+        <v>93.52654967401791</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -863,13 +863,13 @@
         <v>21</v>
       </c>
       <c r="E9">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F9">
         <v>2</v>
       </c>
       <c r="G9">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H9">
         <v>3998</v>
@@ -881,13 +881,13 @@
         <v>2.5</v>
       </c>
       <c r="K9">
-        <v>86.25</v>
+        <v>87.5</v>
       </c>
       <c r="L9">
         <v>99.95</v>
       </c>
       <c r="M9">
-        <v>88.6359913093125</v>
+        <v>89.19308401049261</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -895,31 +895,31 @@
         <v>22</v>
       </c>
       <c r="E10">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F10">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H10">
-        <v>3991</v>
+        <v>3996</v>
       </c>
       <c r="I10">
-        <v>0.225</v>
+        <v>0.1</v>
       </c>
       <c r="J10">
-        <v>11.25</v>
+        <v>5</v>
       </c>
       <c r="K10">
-        <v>95</v>
+        <v>93.75</v>
       </c>
       <c r="L10">
-        <v>99.77500000000001</v>
+        <v>99.90000000000001</v>
       </c>
       <c r="M10">
-        <v>93.03922290903267</v>
+        <v>92.3303127108089</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -951,7 +951,7 @@
         <v>99.825</v>
       </c>
       <c r="M11">
-        <v>89.93776273302899</v>
+        <v>89.83798760613752</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -959,31 +959,31 @@
         <v>24</v>
       </c>
       <c r="E12">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F12">
+        <v>8</v>
+      </c>
+      <c r="G12">
+        <v>15</v>
+      </c>
+      <c r="H12">
+        <v>3992</v>
+      </c>
+      <c r="I12">
+        <v>0.2</v>
+      </c>
+      <c r="J12">
         <v>10</v>
       </c>
-      <c r="G12">
-        <v>14</v>
-      </c>
-      <c r="H12">
-        <v>3990</v>
-      </c>
-      <c r="I12">
-        <v>0.25</v>
-      </c>
-      <c r="J12">
-        <v>12.5</v>
-      </c>
       <c r="K12">
-        <v>82.5</v>
+        <v>81.25</v>
       </c>
       <c r="L12">
-        <v>99.75</v>
+        <v>99.8</v>
       </c>
       <c r="M12">
-        <v>86.61305739558701</v>
+        <v>85.82812778542504</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -991,31 +991,31 @@
         <v>25</v>
       </c>
       <c r="E13">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F13">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H13">
-        <v>3984</v>
+        <v>3986</v>
       </c>
       <c r="I13">
-        <v>0.4</v>
+        <v>0.35</v>
       </c>
       <c r="J13">
-        <v>20</v>
+        <v>17.5</v>
       </c>
       <c r="K13">
-        <v>96.25</v>
+        <v>93.75</v>
       </c>
       <c r="L13">
-        <v>99.59999999999999</v>
+        <v>99.65000000000001</v>
       </c>
       <c r="M13">
-        <v>93.6346910493305</v>
+        <v>92.3303127108089</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -1026,28 +1026,28 @@
         <v>78</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G14">
         <v>2</v>
       </c>
       <c r="H14">
-        <v>4000</v>
+        <v>3997</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>0.075</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>3.75</v>
       </c>
       <c r="K14">
         <v>97.5</v>
       </c>
       <c r="L14">
-        <v>100</v>
+        <v>99.925</v>
       </c>
       <c r="M14">
-        <v>94.22226833776028</v>
+        <v>94.11276627809835</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -1079,7 +1079,7 @@
         <v>99.77500000000001</v>
       </c>
       <c r="M15">
-        <v>86.61305739558701</v>
+        <v>86.5205188481533</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -1087,31 +1087,31 @@
         <v>28</v>
       </c>
       <c r="E16">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F16">
+        <v>4</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="H16">
+        <v>3996</v>
+      </c>
+      <c r="I16">
+        <v>0.1</v>
+      </c>
+      <c r="J16">
         <v>5</v>
       </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16">
-        <v>3995</v>
-      </c>
-      <c r="I16">
-        <v>0.125</v>
-      </c>
-      <c r="J16">
-        <v>6.25</v>
-      </c>
       <c r="K16">
-        <v>98.75</v>
+        <v>97.5</v>
       </c>
       <c r="L16">
-        <v>99.875</v>
+        <v>99.90000000000001</v>
       </c>
       <c r="M16">
-        <v>94.80211059047315</v>
+        <v>94.11276627809835</v>
       </c>
     </row>
     <row r="17" spans="4:13">
@@ -1119,31 +1119,31 @@
         <v>29</v>
       </c>
       <c r="E17">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G17">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="H17">
-        <v>3999</v>
+        <v>3997</v>
       </c>
       <c r="I17">
-        <v>0.025</v>
+        <v>0.075</v>
       </c>
       <c r="J17">
-        <v>1.25</v>
+        <v>3.75</v>
       </c>
       <c r="K17">
-        <v>83.75</v>
+        <v>77.5</v>
       </c>
       <c r="L17">
-        <v>99.97500000000001</v>
+        <v>99.925</v>
       </c>
       <c r="M17">
-        <v>87.29700679951185</v>
+        <v>83.68930020654656</v>
       </c>
     </row>
     <row r="18" spans="4:13">
@@ -1151,31 +1151,31 @@
         <v>30</v>
       </c>
       <c r="E18">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F18">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G18">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H18">
-        <v>3980</v>
+        <v>3982</v>
       </c>
       <c r="I18">
-        <v>0.5</v>
+        <v>0.45</v>
       </c>
       <c r="J18">
-        <v>25</v>
+        <v>22.5</v>
       </c>
       <c r="K18">
-        <v>95</v>
+        <v>92.5</v>
       </c>
       <c r="L18">
-        <v>99.5</v>
+        <v>99.55000000000001</v>
       </c>
       <c r="M18">
-        <v>93.03922290903267</v>
+        <v>91.71996796672292</v>
       </c>
     </row>
     <row r="19" spans="4:13">
@@ -1207,7 +1207,7 @@
         <v>99.97500000000001</v>
       </c>
       <c r="M19">
-        <v>95.37436954802941</v>
+        <v>95.26217484169058</v>
       </c>
     </row>
     <row r="20" spans="4:13">
@@ -1218,28 +1218,28 @@
         <v>80</v>
       </c>
       <c r="F20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
       <c r="H20">
-        <v>3996</v>
+        <v>3997</v>
       </c>
       <c r="I20">
-        <v>0.1</v>
+        <v>0.075</v>
       </c>
       <c r="J20">
-        <v>5</v>
+        <v>3.75</v>
       </c>
       <c r="K20">
         <v>100</v>
       </c>
       <c r="L20">
-        <v>99.90000000000001</v>
+        <v>99.925</v>
       </c>
       <c r="M20">
-        <v>95.37436954802941</v>
+        <v>95.26217484169058</v>
       </c>
     </row>
     <row r="21" spans="4:13">
@@ -1247,13 +1247,13 @@
         <v>33</v>
       </c>
       <c r="E21">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F21">
         <v>10</v>
       </c>
       <c r="G21">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H21">
         <v>3990</v>
@@ -1265,13 +1265,13 @@
         <v>12.5</v>
       </c>
       <c r="K21">
-        <v>97.5</v>
+        <v>95</v>
       </c>
       <c r="L21">
         <v>99.75</v>
       </c>
       <c r="M21">
-        <v>94.22226833776028</v>
+        <v>92.93245182222844</v>
       </c>
     </row>
     <row r="22" spans="4:13">
@@ -1279,31 +1279,31 @@
         <v>34</v>
       </c>
       <c r="E22">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F22">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="G22">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H22">
-        <v>3982</v>
+        <v>3993</v>
       </c>
       <c r="I22">
-        <v>0.45</v>
+        <v>0.175</v>
       </c>
       <c r="J22">
-        <v>22.5</v>
+        <v>8.75</v>
       </c>
       <c r="K22">
-        <v>93.75</v>
+        <v>91.25</v>
       </c>
       <c r="L22">
-        <v>99.55000000000001</v>
+        <v>99.825</v>
       </c>
       <c r="M22">
-        <v>92.4357038873674</v>
+        <v>91.10124870622212</v>
       </c>
     </row>
     <row r="23" spans="4:13">
@@ -1314,28 +1314,28 @@
         <v>78</v>
       </c>
       <c r="F23">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G23">
         <v>2</v>
       </c>
       <c r="H23">
-        <v>3992</v>
+        <v>3993</v>
       </c>
       <c r="I23">
-        <v>0.2</v>
+        <v>0.175</v>
       </c>
       <c r="J23">
-        <v>10</v>
+        <v>8.75</v>
       </c>
       <c r="K23">
         <v>97.5</v>
       </c>
       <c r="L23">
-        <v>99.8</v>
+        <v>99.825</v>
       </c>
       <c r="M23">
-        <v>94.22226833776028</v>
+        <v>94.11276627809835</v>
       </c>
     </row>
     <row r="24" spans="4:13">
@@ -1346,28 +1346,28 @@
         <v>79</v>
       </c>
       <c r="F24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G24">
         <v>1</v>
       </c>
       <c r="H24">
-        <v>3996</v>
+        <v>3995</v>
       </c>
       <c r="I24">
-        <v>0.1</v>
+        <v>0.125</v>
       </c>
       <c r="J24">
-        <v>5</v>
+        <v>6.25</v>
       </c>
       <c r="K24">
         <v>98.75</v>
       </c>
       <c r="L24">
-        <v>99.90000000000001</v>
+        <v>99.875</v>
       </c>
       <c r="M24">
-        <v>94.80211059047315</v>
+        <v>94.69125742895785</v>
       </c>
     </row>
     <row r="25" spans="4:13">
@@ -1375,31 +1375,31 @@
         <v>37</v>
       </c>
       <c r="E25">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F25">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="G25">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H25">
-        <v>3991</v>
+        <v>3984</v>
       </c>
       <c r="I25">
-        <v>0.225</v>
+        <v>0.4</v>
       </c>
       <c r="J25">
-        <v>11.25</v>
+        <v>20</v>
       </c>
       <c r="K25">
-        <v>87.5</v>
+        <v>90</v>
       </c>
       <c r="L25">
-        <v>99.77500000000001</v>
+        <v>99.59999999999999</v>
       </c>
       <c r="M25">
-        <v>89.29143101977752</v>
+        <v>90.47398137904899</v>
       </c>
     </row>
     <row r="26" spans="4:13">
@@ -1407,31 +1407,31 @@
         <v>38</v>
       </c>
       <c r="E26">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F26">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G26">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H26">
-        <v>3997</v>
+        <v>3992</v>
       </c>
       <c r="I26">
-        <v>0.075</v>
+        <v>0.2</v>
       </c>
       <c r="J26">
-        <v>3.75</v>
+        <v>10</v>
       </c>
       <c r="K26">
-        <v>96.25</v>
+        <v>98.75</v>
       </c>
       <c r="L26">
-        <v>99.925</v>
+        <v>99.8</v>
       </c>
       <c r="M26">
-        <v>93.6346910493305</v>
+        <v>94.69125742895785</v>
       </c>
     </row>
     <row r="27" spans="4:13">
@@ -1439,31 +1439,31 @@
         <v>39</v>
       </c>
       <c r="E27">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F27">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G27">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H27">
-        <v>3982</v>
+        <v>3979</v>
       </c>
       <c r="I27">
-        <v>0.45</v>
+        <v>0.525</v>
       </c>
       <c r="J27">
-        <v>22.5</v>
+        <v>26.25</v>
       </c>
       <c r="K27">
-        <v>83.75</v>
+        <v>78.75</v>
       </c>
       <c r="L27">
-        <v>99.55000000000001</v>
+        <v>99.47500000000001</v>
       </c>
       <c r="M27">
-        <v>87.29700679951185</v>
+        <v>84.41274553190017</v>
       </c>
     </row>
     <row r="28" spans="4:13">
@@ -1471,31 +1471,31 @@
         <v>40</v>
       </c>
       <c r="E28">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F28">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G28">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H28">
-        <v>3987</v>
+        <v>3990</v>
       </c>
       <c r="I28">
-        <v>0.325</v>
+        <v>0.25</v>
       </c>
       <c r="J28">
-        <v>16.25</v>
+        <v>12.5</v>
       </c>
       <c r="K28">
-        <v>63.74999999999999</v>
+        <v>61.25000000000001</v>
       </c>
       <c r="L28">
-        <v>99.675</v>
+        <v>99.75</v>
       </c>
       <c r="M28">
-        <v>75.02925496025586</v>
+        <v>73.20316677599722</v>
       </c>
     </row>
     <row r="29" spans="4:13">
@@ -1503,31 +1503,31 @@
         <v>41</v>
       </c>
       <c r="E29">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F29">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H29">
-        <v>3999</v>
+        <v>3997</v>
       </c>
       <c r="I29">
-        <v>0.025</v>
+        <v>0.075</v>
       </c>
       <c r="J29">
-        <v>1.25</v>
+        <v>3.75</v>
       </c>
       <c r="K29">
-        <v>98.75</v>
+        <v>97.5</v>
       </c>
       <c r="L29">
-        <v>99.97500000000001</v>
+        <v>99.925</v>
       </c>
       <c r="M29">
-        <v>94.80211059047315</v>
+        <v>94.11276627809835</v>
       </c>
     </row>
     <row r="30" spans="4:13">
@@ -1535,31 +1535,31 @@
         <v>42</v>
       </c>
       <c r="E30">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F30">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G30">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H30">
-        <v>3992</v>
+        <v>3995</v>
       </c>
       <c r="I30">
-        <v>0.2</v>
+        <v>0.125</v>
       </c>
       <c r="J30">
-        <v>10</v>
+        <v>6.25</v>
       </c>
       <c r="K30">
-        <v>87.5</v>
+        <v>82.5</v>
       </c>
       <c r="L30">
-        <v>99.8</v>
+        <v>99.875</v>
       </c>
       <c r="M30">
-        <v>89.29143101977752</v>
+        <v>86.5205188481533</v>
       </c>
     </row>
     <row r="31" spans="4:13">
@@ -1567,31 +1567,31 @@
         <v>43</v>
       </c>
       <c r="E31">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F31">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G31">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H31">
-        <v>3991</v>
+        <v>3992</v>
       </c>
       <c r="I31">
-        <v>0.225</v>
+        <v>0.2</v>
       </c>
       <c r="J31">
-        <v>11.25</v>
+        <v>10</v>
       </c>
       <c r="K31">
-        <v>98.75</v>
+        <v>96.25</v>
       </c>
       <c r="L31">
-        <v>99.77500000000001</v>
+        <v>99.8</v>
       </c>
       <c r="M31">
-        <v>94.80211059047315</v>
+        <v>93.52654967401791</v>
       </c>
     </row>
     <row r="32" spans="4:13">
@@ -1623,7 +1623,7 @@
         <v>99.97500000000001</v>
       </c>
       <c r="M32">
-        <v>95.37436954802941</v>
+        <v>95.26217484169058</v>
       </c>
     </row>
     <row r="33" spans="4:13">
@@ -1631,31 +1631,31 @@
         <v>45</v>
       </c>
       <c r="E33">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="F33">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G33">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H33">
-        <v>3993</v>
+        <v>3987</v>
       </c>
       <c r="I33">
-        <v>0.175</v>
+        <v>0.325</v>
       </c>
       <c r="J33">
-        <v>8.75</v>
+        <v>16.25</v>
       </c>
       <c r="K33">
-        <v>77.5</v>
+        <v>83.75</v>
       </c>
       <c r="L33">
-        <v>99.825</v>
+        <v>99.675</v>
       </c>
       <c r="M33">
-        <v>83.77587851988477</v>
+        <v>87.20300179345281</v>
       </c>
     </row>
     <row r="34" spans="4:13">
@@ -1663,31 +1663,31 @@
         <v>46</v>
       </c>
       <c r="E34">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F34">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G34">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H34">
-        <v>3993</v>
+        <v>3992</v>
       </c>
       <c r="I34">
-        <v>0.175</v>
+        <v>0.2</v>
       </c>
       <c r="J34">
-        <v>8.75</v>
+        <v>10</v>
       </c>
       <c r="K34">
-        <v>91.25</v>
+        <v>95</v>
       </c>
       <c r="L34">
-        <v>99.825</v>
+        <v>99.8</v>
       </c>
       <c r="M34">
-        <v>91.20385114900078</v>
+        <v>92.93245182222844</v>
       </c>
     </row>
     <row r="35" spans="4:13">
@@ -1698,28 +1698,28 @@
         <v>76</v>
       </c>
       <c r="F35">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G35">
         <v>4</v>
       </c>
       <c r="H35">
-        <v>3997</v>
+        <v>3999</v>
       </c>
       <c r="I35">
-        <v>0.075</v>
+        <v>0.025</v>
       </c>
       <c r="J35">
-        <v>3.75</v>
+        <v>1.25</v>
       </c>
       <c r="K35">
         <v>95</v>
       </c>
       <c r="L35">
-        <v>99.925</v>
+        <v>99.97500000000001</v>
       </c>
       <c r="M35">
-        <v>93.03922290903267</v>
+        <v>92.93245182222844</v>
       </c>
     </row>
     <row r="36" spans="4:13">
@@ -1727,31 +1727,31 @@
         <v>48</v>
       </c>
       <c r="E36">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F36">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="G36">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H36">
-        <v>3988</v>
+        <v>3994</v>
       </c>
       <c r="I36">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="J36">
-        <v>15</v>
+        <v>7.5</v>
       </c>
       <c r="K36">
-        <v>96.25</v>
+        <v>97.5</v>
       </c>
       <c r="L36">
-        <v>99.7</v>
+        <v>99.85000000000001</v>
       </c>
       <c r="M36">
-        <v>93.6346910493305</v>
+        <v>94.11276627809835</v>
       </c>
     </row>
     <row r="37" spans="4:13">
@@ -1759,31 +1759,31 @@
         <v>49</v>
       </c>
       <c r="E37">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F37">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G37">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H37">
-        <v>3991</v>
+        <v>3992</v>
       </c>
       <c r="I37">
-        <v>0.225</v>
+        <v>0.2</v>
       </c>
       <c r="J37">
-        <v>11.25</v>
+        <v>10</v>
       </c>
       <c r="K37">
-        <v>90</v>
+        <v>92.5</v>
       </c>
       <c r="L37">
-        <v>99.77500000000001</v>
+        <v>99.8</v>
       </c>
       <c r="M37">
-        <v>90.57517498634861</v>
+        <v>91.71996796672292</v>
       </c>
     </row>
     <row r="38" spans="4:13">
@@ -1794,28 +1794,28 @@
         <v>75</v>
       </c>
       <c r="F38">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G38">
         <v>5</v>
       </c>
       <c r="H38">
-        <v>3998</v>
+        <v>3996</v>
       </c>
       <c r="I38">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="J38">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="K38">
         <v>93.75</v>
       </c>
       <c r="L38">
-        <v>99.95</v>
+        <v>99.90000000000001</v>
       </c>
       <c r="M38">
-        <v>92.4357038873674</v>
+        <v>92.3303127108089</v>
       </c>
     </row>
     <row r="39" spans="4:13">
@@ -1826,28 +1826,28 @@
         <v>80</v>
       </c>
       <c r="F39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G39">
         <v>0</v>
       </c>
       <c r="H39">
-        <v>4000</v>
+        <v>3999</v>
       </c>
       <c r="I39">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="J39">
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="K39">
         <v>100</v>
       </c>
       <c r="L39">
-        <v>100</v>
+        <v>99.97500000000001</v>
       </c>
       <c r="M39">
-        <v>95.37436954802941</v>
+        <v>95.26217484169058</v>
       </c>
     </row>
     <row r="40" spans="4:13">
@@ -1855,13 +1855,13 @@
         <v>52</v>
       </c>
       <c r="E40">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F40">
         <v>5</v>
       </c>
       <c r="G40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H40">
         <v>3995</v>
@@ -1873,13 +1873,13 @@
         <v>6.25</v>
       </c>
       <c r="K40">
-        <v>98.75</v>
+        <v>97.5</v>
       </c>
       <c r="L40">
         <v>99.875</v>
       </c>
       <c r="M40">
-        <v>94.80211059047315</v>
+        <v>94.11276627809835</v>
       </c>
     </row>
     <row r="41" spans="4:13">
@@ -1887,31 +1887,31 @@
         <v>53</v>
       </c>
       <c r="E41">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F41">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G41">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H41">
-        <v>3992</v>
+        <v>3990</v>
       </c>
       <c r="I41">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="J41">
-        <v>10</v>
+        <v>12.5</v>
       </c>
       <c r="K41">
-        <v>86.25</v>
+        <v>88.75</v>
       </c>
       <c r="L41">
-        <v>99.8</v>
+        <v>99.75</v>
       </c>
       <c r="M41">
-        <v>88.6359913093125</v>
+        <v>89.83798760613752</v>
       </c>
     </row>
     <row r="42" spans="4:13">
@@ -1919,31 +1919,31 @@
         <v>54</v>
       </c>
       <c r="E42">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F42">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G42">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H42">
-        <v>3992</v>
+        <v>3989</v>
       </c>
       <c r="I42">
-        <v>0.2</v>
+        <v>0.275</v>
       </c>
       <c r="J42">
-        <v>10</v>
+        <v>13.75</v>
       </c>
       <c r="K42">
-        <v>88.75</v>
+        <v>93.75</v>
       </c>
       <c r="L42">
-        <v>99.8</v>
+        <v>99.72499999999999</v>
       </c>
       <c r="M42">
-        <v>89.93776273302899</v>
+        <v>92.3303127108089</v>
       </c>
     </row>
     <row r="43" spans="4:13">
@@ -1951,13 +1951,13 @@
         <v>55</v>
       </c>
       <c r="E43">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F43">
         <v>11</v>
       </c>
       <c r="G43">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H43">
         <v>3989</v>
@@ -1969,13 +1969,13 @@
         <v>13.75</v>
       </c>
       <c r="K43">
-        <v>85</v>
+        <v>86.25</v>
       </c>
       <c r="L43">
         <v>99.72499999999999</v>
       </c>
       <c r="M43">
-        <v>87.97124971297588</v>
+        <v>88.53908204091192</v>
       </c>
     </row>
     <row r="44" spans="4:13">
@@ -1986,28 +1986,28 @@
         <v>79</v>
       </c>
       <c r="F44">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G44">
         <v>1</v>
       </c>
       <c r="H44">
-        <v>3994</v>
+        <v>3993</v>
       </c>
       <c r="I44">
-        <v>0.15</v>
+        <v>0.175</v>
       </c>
       <c r="J44">
-        <v>7.5</v>
+        <v>8.75</v>
       </c>
       <c r="K44">
         <v>98.75</v>
       </c>
       <c r="L44">
-        <v>99.85000000000001</v>
+        <v>99.825</v>
       </c>
       <c r="M44">
-        <v>94.80211059047315</v>
+        <v>94.69125742895785</v>
       </c>
     </row>
     <row r="45" spans="4:13">
@@ -2015,31 +2015,31 @@
         <v>57</v>
       </c>
       <c r="E45">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F45">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G45">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H45">
-        <v>3993</v>
+        <v>3990</v>
       </c>
       <c r="I45">
-        <v>0.175</v>
+        <v>0.25</v>
       </c>
       <c r="J45">
-        <v>8.75</v>
+        <v>12.5</v>
       </c>
       <c r="K45">
-        <v>90</v>
+        <v>86.25</v>
       </c>
       <c r="L45">
-        <v>99.825</v>
+        <v>99.75</v>
       </c>
       <c r="M45">
-        <v>90.57517498634861</v>
+        <v>88.53908204091192</v>
       </c>
     </row>
     <row r="46" spans="4:13">
@@ -2047,31 +2047,31 @@
         <v>58</v>
       </c>
       <c r="E46">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F46">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G46">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H46">
-        <v>4000</v>
+        <v>3998</v>
       </c>
       <c r="I46">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="J46">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="K46">
-        <v>81.25</v>
+        <v>82.5</v>
       </c>
       <c r="L46">
-        <v>100</v>
+        <v>99.95</v>
       </c>
       <c r="M46">
-        <v>85.91919037763267</v>
+        <v>86.5205188481533</v>
       </c>
     </row>
     <row r="47" spans="4:13">
@@ -2079,13 +2079,13 @@
         <v>59</v>
       </c>
       <c r="E47">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F47">
         <v>0</v>
       </c>
       <c r="G47">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H47">
         <v>4000</v>
@@ -2097,13 +2097,13 @@
         <v>0</v>
       </c>
       <c r="K47">
-        <v>97.5</v>
+        <v>96.25</v>
       </c>
       <c r="L47">
         <v>100</v>
       </c>
       <c r="M47">
-        <v>94.22226833776028</v>
+        <v>93.52654967401791</v>
       </c>
     </row>
     <row r="48" spans="4:13">
@@ -2111,31 +2111,31 @@
         <v>60</v>
       </c>
       <c r="E48">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F48">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G48">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H48">
-        <v>3998</v>
+        <v>3997</v>
       </c>
       <c r="I48">
-        <v>0.05</v>
+        <v>0.075</v>
       </c>
       <c r="J48">
-        <v>2.5</v>
+        <v>3.75</v>
       </c>
       <c r="K48">
-        <v>98.75</v>
+        <v>96.25</v>
       </c>
       <c r="L48">
-        <v>99.95</v>
+        <v>99.925</v>
       </c>
       <c r="M48">
-        <v>94.80211059047315</v>
+        <v>93.52654967401791</v>
       </c>
     </row>
     <row r="49" spans="4:13">
@@ -2143,13 +2143,13 @@
         <v>61</v>
       </c>
       <c r="E49">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F49">
         <v>3</v>
       </c>
       <c r="G49">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H49">
         <v>3997</v>
@@ -2161,13 +2161,13 @@
         <v>3.75</v>
       </c>
       <c r="K49">
-        <v>86.25</v>
+        <v>87.5</v>
       </c>
       <c r="L49">
         <v>99.925</v>
       </c>
       <c r="M49">
-        <v>88.6359913093125</v>
+        <v>89.19308401049261</v>
       </c>
     </row>
     <row r="50" spans="4:13">
@@ -2175,31 +2175,31 @@
         <v>62</v>
       </c>
       <c r="E50">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G50">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H50">
-        <v>3999</v>
+        <v>4000</v>
       </c>
       <c r="I50">
-        <v>0.025</v>
+        <v>0</v>
       </c>
       <c r="J50">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="K50">
-        <v>92.5</v>
+        <v>91.25</v>
       </c>
       <c r="L50">
-        <v>99.97500000000001</v>
+        <v>100</v>
       </c>
       <c r="M50">
-        <v>91.82396959810377</v>
+        <v>91.10124870622212</v>
       </c>
     </row>
     <row r="51" spans="4:13">
@@ -2207,31 +2207,31 @@
         <v>63</v>
       </c>
       <c r="E51">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F51">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G51">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H51">
-        <v>3994</v>
+        <v>3990</v>
       </c>
       <c r="I51">
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
       <c r="J51">
-        <v>7.5</v>
+        <v>12.5</v>
       </c>
       <c r="K51">
-        <v>85</v>
+        <v>87.5</v>
       </c>
       <c r="L51">
-        <v>99.85000000000001</v>
+        <v>99.75</v>
       </c>
       <c r="M51">
-        <v>87.97124971297588</v>
+        <v>89.19308401049261</v>
       </c>
     </row>
     <row r="52" spans="4:13">
@@ -2239,31 +2239,31 @@
         <v>64</v>
       </c>
       <c r="E52">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F52">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G52">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H52">
-        <v>3991</v>
+        <v>3995</v>
       </c>
       <c r="I52">
-        <v>0.225</v>
+        <v>0.125</v>
       </c>
       <c r="J52">
-        <v>11.25</v>
+        <v>6.25</v>
       </c>
       <c r="K52">
-        <v>83.75</v>
+        <v>81.25</v>
       </c>
       <c r="L52">
-        <v>99.77500000000001</v>
+        <v>99.875</v>
       </c>
       <c r="M52">
-        <v>87.29700679951185</v>
+        <v>85.82812778542504</v>
       </c>
     </row>
   </sheetData>

</xml_diff>